<commit_message>
Journal entry and Account Payable TC
</commit_message>
<xml_diff>
--- a/templates/QARSF/Account Payable.xlsx
+++ b/templates/QARSF/Account Payable.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ErpFinalProject\rsqasampleproj\rsqasampleproj\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28823EAE-BB28-465D-8214-D2C68D863DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F87D8CC-0BCA-4FD0-93BE-F16EAC406039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
     <sheet name="BankDetail" sheetId="16" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId3"/>
+    <sheet name="JournalEntriesD" sheetId="18" r:id="rId4"/>
+    <sheet name="JournalEntries" sheetId="19" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Vendor</t>
   </si>
@@ -59,6 +62,54 @@
   </si>
   <si>
     <t>a9d1K0000004DGVQA2</t>
+  </si>
+  <si>
+    <t>CloseTransaction</t>
+  </si>
+  <si>
+    <t>PostTransaction</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Paytype</t>
+  </si>
+  <si>
+    <t>EFT</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>DebitAmount</t>
+  </si>
+  <si>
+    <t>CreditAmount</t>
+  </si>
+  <si>
+    <t>Reversal</t>
+  </si>
+  <si>
+    <t>6622 (Cash Account)</t>
+  </si>
+  <si>
+    <t>1100 (Accounts Receivable Trade)</t>
+  </si>
+  <si>
+    <t>EntryDesc</t>
+  </si>
+  <si>
+    <t>NPAUTOTest</t>
+  </si>
+  <si>
+    <t>NPAUTOTestRev</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BankAccount</t>
   </si>
 </sst>
 </file>
@@ -94,9 +145,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D721CDB-A9DB-40A7-92FA-BE728EC43FA8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,9 +477,11 @@
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +491,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -445,6 +513,18 @@
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -455,10 +535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED581F5-27B1-42C4-BD3E-B23B453B4E89}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,13 +556,137 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEC8942-3B81-4719-B47B-7D8E287A86DD}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF28B4E6-0495-4E52-B25E-8C3A3E173311}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7E54B2-B7B4-44D4-8D7C-1B0233FCC129}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
General Ledger Test Cases
</commit_message>
<xml_diff>
--- a/templates/QARSF/Account Payable.xlsx
+++ b/templates/QARSF/Account Payable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F87D8CC-0BCA-4FD0-93BE-F16EAC406039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F9BBF0-CBB3-45AD-B265-C7A75A636D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="6" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="Sheet1" sheetId="17" r:id="rId3"/>
     <sheet name="JournalEntriesD" sheetId="18" r:id="rId4"/>
     <sheet name="JournalEntries" sheetId="19" r:id="rId5"/>
+    <sheet name="GLAccount" sheetId="20" r:id="rId6"/>
+    <sheet name="APATO" sheetId="21" r:id="rId7"/>
+    <sheet name="PAYTO" sheetId="23" r:id="rId8"/>
+    <sheet name="ObjectName" sheetId="22" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="57">
   <si>
     <t>Vendor</t>
   </si>
@@ -52,9 +56,6 @@
     <t>Invoice</t>
   </si>
   <si>
-    <t>NPTestAuto (1146)</t>
-  </si>
-  <si>
     <t>Bank Account</t>
   </si>
   <si>
@@ -110,19 +111,127 @@
   </si>
   <si>
     <t>BankAccount</t>
+  </si>
+  <si>
+    <t>GLAccountName</t>
+  </si>
+  <si>
+    <t>NPTestGLTXN (2601)</t>
+  </si>
+  <si>
+    <t>AmountBefore</t>
+  </si>
+  <si>
+    <t>AmountAfter</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Fiscalyear</t>
+  </si>
+  <si>
+    <t>PayType</t>
+  </si>
+  <si>
+    <t>GLAccount</t>
+  </si>
+  <si>
+    <t>Mountain Manufacturing (100)</t>
+  </si>
+  <si>
+    <t>6655 (BC)</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>SB-24808 (1103)</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>PostPayTrans</t>
+  </si>
+  <si>
+    <t>Vendor Credit</t>
+  </si>
+  <si>
+    <t>Vendor Debit</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>Bank of Dad</t>
+  </si>
+  <si>
+    <t>2602 (Accounts Payable)</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>Dim1</t>
+  </si>
+  <si>
+    <t>Dim2</t>
+  </si>
+  <si>
+    <t>Dim3</t>
+  </si>
+  <si>
+    <t>Dim4</t>
+  </si>
+  <si>
+    <t>DimVal</t>
+  </si>
+  <si>
+    <t>Red Widgets</t>
+  </si>
+  <si>
+    <t>DIV11</t>
+  </si>
+  <si>
+    <t>TEST3</t>
+  </si>
+  <si>
+    <t>Green Widgets</t>
+  </si>
+  <si>
+    <t>Red Widgets|DIV11|TEST3|Green Widgets||||</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,12 +254,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,23 +576,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D721CDB-A9DB-40A7-92FA-BE728EC43FA8}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,21 +604,24 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -515,16 +630,19 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -538,22 +656,22 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -572,22 +690,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -600,30 +718,30 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -634,7 +752,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -659,31 +777,750 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BBAF44-E262-4A71-B8CF-10422D312420}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6332D76E-5850-479F-B02D-9B6334D6ED9C}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2">
+        <v>2022</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3">
+        <v>2022</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>2022</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8">
+        <v>2022</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9">
+        <v>2022</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10">
+        <v>2022</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11">
+        <v>2022</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12">
+        <v>2022</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>35</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13">
+        <v>2022</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C24426-28EA-4B2B-B07E-16C17FE8A617}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>460</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2">
+        <v>2022</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1218322B-C8F8-4601-8448-6FB48136F898}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GL Transaction Verification and Already Posted APINV
</commit_message>
<xml_diff>
--- a/templates/QARSF/Account Payable.xlsx
+++ b/templates/QARSF/Account Payable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F9BBF0-CBB3-45AD-B265-C7A75A636D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F55689C-FA9C-48A9-A3C6-B739A308E79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="6" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="4" activeTab="7" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="15" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="JournalEntries" sheetId="19" r:id="rId5"/>
     <sheet name="GLAccount" sheetId="20" r:id="rId6"/>
     <sheet name="APATO" sheetId="21" r:id="rId7"/>
-    <sheet name="PAYTO" sheetId="23" r:id="rId8"/>
-    <sheet name="ObjectName" sheetId="22" r:id="rId9"/>
+    <sheet name="APATO_ForeignCurr" sheetId="24" r:id="rId8"/>
+    <sheet name="PAYTO" sheetId="23" r:id="rId9"/>
+    <sheet name="ObjectName" sheetId="22" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="59">
   <si>
     <t>Vendor</t>
   </si>
@@ -213,6 +214,12 @@
   </si>
   <si>
     <t>Red Widgets|DIV11|TEST3|Green Widgets||||</t>
+  </si>
+  <si>
+    <t>LoadPosted</t>
+  </si>
+  <si>
+    <t>BC Vendor INR (1097)</t>
   </si>
 </sst>
 </file>
@@ -651,6 +658,62 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1218322B-C8F8-4601-8448-6FB48136F898}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2">
+        <v>2022</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED581F5-27B1-42C4-BD3E-B23B453B4E89}">
   <dimension ref="A1:A2"/>
@@ -889,10 +952,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6332D76E-5850-479F-B02D-9B6334D6ED9C}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,12 +965,13 @@
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -939,22 +1003,25 @@
         <v>40</v>
       </c>
       <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
         <v>47</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>48</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -971,7 +1038,7 @@
         <v>37</v>
       </c>
       <c r="F2">
-        <v>35</v>
+        <v>650</v>
       </c>
       <c r="G2" t="s">
         <v>38</v>
@@ -983,25 +1050,13 @@
         <v>3</v>
       </c>
       <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -1018,7 +1073,7 @@
         <v>37</v>
       </c>
       <c r="F3">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -1030,10 +1085,28 @@
         <v>3</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1050,7 +1123,7 @@
         <v>37</v>
       </c>
       <c r="F4">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G4" t="s">
         <v>38</v>
@@ -1059,28 +1132,16 @@
         <v>2022</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1097,7 +1158,7 @@
         <v>37</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G5" t="s">
         <v>38</v>
@@ -1109,10 +1170,28 @@
         <v>41</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1129,7 +1208,7 @@
         <v>37</v>
       </c>
       <c r="F6">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G6" t="s">
         <v>38</v>
@@ -1138,28 +1217,16 @@
         <v>2022</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1176,7 +1243,7 @@
         <v>37</v>
       </c>
       <c r="F7">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G7" t="s">
         <v>38</v>
@@ -1188,10 +1255,28 @@
         <v>42</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1208,22 +1293,25 @@
         <v>37</v>
       </c>
       <c r="F8">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8">
         <v>2022</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1240,7 +1328,7 @@
         <v>37</v>
       </c>
       <c r="F9">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G9" t="s">
         <v>39</v>
@@ -1252,10 +1340,13 @@
         <v>3</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1272,7 +1363,7 @@
         <v>37</v>
       </c>
       <c r="F10">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G10" t="s">
         <v>39</v>
@@ -1281,13 +1372,16 @@
         <v>2022</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1304,7 +1398,7 @@
         <v>37</v>
       </c>
       <c r="F11">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G11" t="s">
         <v>39</v>
@@ -1316,10 +1410,13 @@
         <v>41</v>
       </c>
       <c r="J11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -1336,7 +1433,7 @@
         <v>37</v>
       </c>
       <c r="F12">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G12" t="s">
         <v>39</v>
@@ -1345,13 +1442,16 @@
         <v>2022</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1368,7 +1468,7 @@
         <v>37</v>
       </c>
       <c r="F13">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G13" t="s">
         <v>39</v>
@@ -1380,7 +1480,45 @@
         <v>42</v>
       </c>
       <c r="J13" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14">
+        <v>300</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14">
+        <v>2022</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1390,6 +1528,575 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36413420-38E2-48A4-9DB9-E6F8F8778C17}">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2">
+        <v>650</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2">
+        <v>2022</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3">
+        <v>2022</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4">
+        <v>300</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>300</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>2022</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6">
+        <v>300</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>2022</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7">
+        <v>300</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>2022</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8">
+        <v>2022</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9">
+        <v>300</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9">
+        <v>2022</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10">
+        <v>300</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10">
+        <v>2022</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11">
+        <v>300</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11">
+        <v>2022</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12">
+        <v>300</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12">
+        <v>2022</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13">
+        <v>300</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13">
+        <v>2022</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>300</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14">
+        <v>2022</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C24426-28EA-4B2B-B07E-16C17FE8A617}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1470,60 +2177,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1218322B-C8F8-4601-8448-6FB48136F898}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2">
-        <v>2022</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>